<commit_message>
Apply 2022 may data
</commit_message>
<xml_diff>
--- a/Climate/MonthlyAvg/monthlyData.xlsx
+++ b/Climate/MonthlyAvg/monthlyData.xlsx
@@ -1,36 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GittHub\climate\Climate\MonthlyAvg\bin\Debug\net5.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GittHub\climate\Climate\MonthlyAvg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D4C2CB65-69A4-4BBF-A6BD-BCA2E40958C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82DC741-BB14-419E-94F1-7BB6D15EA515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000"/>
+    <workbookView xWindow="-16965" yWindow="1590" windowWidth="14400" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="monthlyData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">monthlyData!$A$1:$C$16</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">monthlyData!$D$1:$D$16</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">monthlyData!$E$1:$E$16</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">monthlyData!$F$1:$F$16</definedName>
-  </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -742,9 +743,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>monthlyData!$C$1:$C$16</c:f>
+              <c:f>monthlyData!$C$1:$C$17</c:f>
               <c:strCache>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>2021 1</c:v>
                 </c:pt>
@@ -792,16 +793,19 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>2022 4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2022 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>monthlyData!$D$1:$D$16</c:f>
+              <c:f>monthlyData!$D$1:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>1.9</c:v>
                 </c:pt>
@@ -848,7 +852,10 @@
                   <c:v>6.1</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9</c:v>
+                  <c:v>10.199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>18.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1188,9 +1195,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>monthlyData!$C$1:$C$16</c:f>
+              <c:f>monthlyData!$C$1:$C$17</c:f>
               <c:strCache>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>2021 1</c:v>
                 </c:pt>
@@ -1238,16 +1245,19 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>2022 4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2022 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>monthlyData!$E$1:$E$16</c:f>
+              <c:f>monthlyData!$E$1:$E$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>1012.7</c:v>
                 </c:pt>
@@ -1294,7 +1304,10 @@
                   <c:v>1026.2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1012.4</c:v>
+                  <c:v>1013.3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1017.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1601,9 +1614,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>monthlyData!$C$1:$C$16</c:f>
+              <c:f>monthlyData!$C$1:$C$17</c:f>
               <c:strCache>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>2021 1</c:v>
                 </c:pt>
@@ -1651,16 +1664,19 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>2022 4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2022 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>monthlyData!$F$1:$F$16</c:f>
+              <c:f>monthlyData!$F$1:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>15</c:v>
                 </c:pt>
@@ -1707,7 +1723,10 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>59</c:v>
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4084,11 +4103,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" topLeftCell="E13" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4122,7 +4141,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="str">
-        <f t="shared" ref="C2:C16" si="0">_xlfn.CONCAT(A2," ",B2)</f>
+        <f t="shared" ref="C2:C17" si="0">_xlfn.CONCAT(A2," ",B2)</f>
         <v>2021 2</v>
       </c>
       <c r="D2">
@@ -4420,13 +4439,34 @@
         <v>2022 4</v>
       </c>
       <c r="D16">
-        <v>9</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="E16">
-        <v>1012.4</v>
+        <v>1013.3</v>
       </c>
       <c r="F16">
-        <v>59</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2022</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>2022 5</v>
+      </c>
+      <c r="D17">
+        <v>18.5</v>
+      </c>
+      <c r="E17">
+        <v>1017.9</v>
+      </c>
+      <c r="F17">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Close year 2022 and change to net6
</commit_message>
<xml_diff>
--- a/Climate/MonthlyAvg/monthlyData.xlsx
+++ b/Climate/MonthlyAvg/monthlyData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GittHub\climate\Climate\MonthlyAvg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82DC741-BB14-419E-94F1-7BB6D15EA515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C9C5E6C-534D-449C-AE83-F026E1693E0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16965" yWindow="1590" windowWidth="14400" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="monthlyData" sheetId="1" r:id="rId1"/>
@@ -743,9 +743,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>monthlyData!$C$1:$C$17</c:f>
+              <c:f>monthlyData!$C$1:$C$24</c:f>
               <c:strCache>
-                <c:ptCount val="17"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>2021 1</c:v>
                 </c:pt>
@@ -796,16 +796,37 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>2022 5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2022 6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2022 7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2022 8</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2022 9</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2022 10</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2022 11</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2022 12</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>monthlyData!$D$1:$D$17</c:f>
+              <c:f>monthlyData!$D$1:$D$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>1.9</c:v>
                 </c:pt>
@@ -856,6 +877,27 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>18.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>23.2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>24.8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>24.6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>15.9</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>12.7</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1105,7 +1147,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.0555555555555555E-2"/>
+          <c:y val="0.21747703412073491"/>
+          <c:w val="0.93888888888888888"/>
+          <c:h val="0.64741506270049576"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -1195,9 +1247,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>monthlyData!$C$1:$C$17</c:f>
+              <c:f>monthlyData!$C$1:$C$24</c:f>
               <c:strCache>
-                <c:ptCount val="17"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>2021 1</c:v>
                 </c:pt>
@@ -1248,16 +1300,37 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>2022 5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2022 6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2022 7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2022 8</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2022 9</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2022 10</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2022 11</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2022 12</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>monthlyData!$E$1:$E$17</c:f>
+              <c:f>monthlyData!$E$1:$E$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>1012.7</c:v>
                 </c:pt>
@@ -1308,6 +1381,27 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>1017.9</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1015.3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1017</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1014</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1013.6</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1023.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1018.5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1019.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1614,9 +1708,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>monthlyData!$C$1:$C$17</c:f>
+              <c:f>monthlyData!$C$1:$C$24</c:f>
               <c:strCache>
-                <c:ptCount val="17"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>2021 1</c:v>
                 </c:pt>
@@ -1667,16 +1761,37 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>2022 5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2022 6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2022 7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2022 8</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2022 9</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2022 10</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2022 11</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2022 12</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>monthlyData!$F$1:$F$17</c:f>
+              <c:f>monthlyData!$F$1:$F$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>15</c:v>
                 </c:pt>
@@ -1727,6 +1842,27 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>80</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3698,16 +3834,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>266699</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>371474</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3735,15 +3871,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:colOff>85724</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>4761</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>209549</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3770,16 +3906,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>61911</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4104,10 +4240,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E13" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="AB24" sqref="AB24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4141,7 +4277,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="str">
-        <f t="shared" ref="C2:C17" si="0">_xlfn.CONCAT(A2," ",B2)</f>
+        <f t="shared" ref="C2:C24" si="0">_xlfn.CONCAT(A2," ",B2)</f>
         <v>2021 2</v>
       </c>
       <c r="D2">
@@ -4467,6 +4603,153 @@
       </c>
       <c r="F17">
         <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2022</v>
+      </c>
+      <c r="B18">
+        <v>6</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>2022 6</v>
+      </c>
+      <c r="D18">
+        <v>23.2</v>
+      </c>
+      <c r="E18">
+        <v>1015.3</v>
+      </c>
+      <c r="F18">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2022</v>
+      </c>
+      <c r="B19">
+        <v>7</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>2022 7</v>
+      </c>
+      <c r="D19">
+        <v>24.8</v>
+      </c>
+      <c r="E19">
+        <v>1017</v>
+      </c>
+      <c r="F19">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2022</v>
+      </c>
+      <c r="B20">
+        <v>8</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>2022 8</v>
+      </c>
+      <c r="D20">
+        <v>24.6</v>
+      </c>
+      <c r="E20">
+        <v>1014</v>
+      </c>
+      <c r="F20">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2022</v>
+      </c>
+      <c r="B21">
+        <v>9</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>2022 9</v>
+      </c>
+      <c r="D21">
+        <v>15.9</v>
+      </c>
+      <c r="E21">
+        <v>1013.6</v>
+      </c>
+      <c r="F21">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2022</v>
+      </c>
+      <c r="B22">
+        <v>10</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>2022 10</v>
+      </c>
+      <c r="D22">
+        <v>12.7</v>
+      </c>
+      <c r="E22">
+        <v>1023.5</v>
+      </c>
+      <c r="F22">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2022</v>
+      </c>
+      <c r="B23">
+        <v>11</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>2022 11</v>
+      </c>
+      <c r="D23">
+        <v>6.5</v>
+      </c>
+      <c r="E23">
+        <v>1018.5</v>
+      </c>
+      <c r="F23">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2022</v>
+      </c>
+      <c r="B24">
+        <v>12</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>2022 12</v>
+      </c>
+      <c r="D24">
+        <v>2.5</v>
+      </c>
+      <c r="E24">
+        <v>1019.2</v>
+      </c>
+      <c r="F24">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>